<commit_message>
Power BI - Practice
</commit_message>
<xml_diff>
--- a/01-interface/Assignm1.xlsx
+++ b/01-interface/Assignm1.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SNikitenko\Desktop\Book\Training\PowerBI\Datas\Assignments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Power BI - Course\01-interface\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA40E66-3DDD-4FE1-A42A-1AB3BC10F865}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12768" xr2:uid="{252D3175-C7D1-45E7-840F-45C8B420D725}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12768"/>
   </bookViews>
   <sheets>
     <sheet name="Отрасли" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="155">
   <si>
     <t>Егоров Мирослав</t>
   </si>
@@ -487,12 +486,21 @@
   </si>
   <si>
     <t>Номер</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Архипов Станислав </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Струна Марина </t>
+  </si>
+  <si>
+    <t>Седов Станислав</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -867,11 +875,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BF878FA-4F13-4AA2-BD21-1660107AA145}">
-  <dimension ref="A1:C141"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C144"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="B143" sqref="B143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2432,6 +2440,39 @@
         <v>146</v>
       </c>
     </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A142" s="3">
+        <v>141</v>
+      </c>
+      <c r="B142" t="s">
+        <v>152</v>
+      </c>
+      <c r="C142" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A143" s="3">
+        <v>142</v>
+      </c>
+      <c r="B143" t="s">
+        <v>153</v>
+      </c>
+      <c r="C143" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A144" s="3">
+        <v>143</v>
+      </c>
+      <c r="B144" t="s">
+        <v>154</v>
+      </c>
+      <c r="C144" t="s">
+        <v>143</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>